<commit_message>
Add ErrorCode service implementation
</commit_message>
<xml_diff>
--- a/system_code/src/main/resources/ErrorCode.xlsx
+++ b/system_code/src/main/resources/ErrorCode.xlsx
@@ -578,7 +578,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -639,6 +639,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1002</v>
+      </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -650,6 +653,9 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1003</v>
+      </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -664,6 +670,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1004</v>
+      </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -678,6 +687,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1005</v>
+      </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -692,6 +704,9 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1006</v>
+      </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -703,6 +718,9 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1007</v>
+      </c>
       <c r="B9" t="s">
         <v>24</v>
       </c>
@@ -717,6 +735,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1008</v>
+      </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
@@ -728,6 +749,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1009</v>
+      </c>
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -739,6 +763,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1010</v>
+      </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
@@ -750,6 +777,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1011</v>
+      </c>
       <c r="B13" t="s">
         <v>33</v>
       </c>
@@ -761,6 +791,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1012</v>
+      </c>
       <c r="B14" t="s">
         <v>35</v>
       </c>
@@ -772,6 +805,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1013</v>
+      </c>
       <c r="B15" t="s">
         <v>37</v>
       </c>
@@ -783,6 +819,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1014</v>
+      </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
@@ -793,7 +832,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1015</v>
+      </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
@@ -804,7 +846,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1016</v>
+      </c>
       <c r="B18" t="s">
         <v>43</v>
       </c>
@@ -815,7 +860,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1017</v>
+      </c>
       <c r="B19" t="s">
         <v>45</v>
       </c>
@@ -826,7 +874,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1018</v>
+      </c>
       <c r="B20" t="s">
         <v>47</v>
       </c>
@@ -837,7 +888,10 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1019</v>
+      </c>
       <c r="B21" t="s">
         <v>49</v>
       </c>
@@ -848,7 +902,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>1020</v>
+      </c>
       <c r="B22" t="s">
         <v>51</v>
       </c>
@@ -859,7 +916,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1021</v>
+      </c>
       <c r="B23" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Optimize the error-code definition.
</commit_message>
<xml_diff>
--- a/system_code/src/main/resources/ErrorCode.xlsx
+++ b/system_code/src/main/resources/ErrorCode.xlsx
@@ -29,10 +29,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>group</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -250,6 +246,10 @@
   </si>
   <si>
     <t>search</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -578,7 +578,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -595,13 +595,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -612,13 +612,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,16 +626,16 @@
         <v>1001</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -643,13 +643,13 @@
         <v>1002</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -657,16 +657,16 @@
         <v>1003</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
       <c r="E5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -674,16 +674,16 @@
         <v>1004</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>14</v>
-      </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -691,16 +691,16 @@
         <v>1005</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -708,13 +708,13 @@
         <v>1006</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -722,16 +722,16 @@
         <v>1007</v>
       </c>
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,13 +739,13 @@
         <v>1008</v>
       </c>
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -753,13 +753,13 @@
         <v>1009</v>
       </c>
       <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -767,13 +767,13 @@
         <v>1010</v>
       </c>
       <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" t="s">
         <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -781,13 +781,13 @@
         <v>1011</v>
       </c>
       <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -795,13 +795,13 @@
         <v>1012</v>
       </c>
       <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
         <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -809,13 +809,13 @@
         <v>1013</v>
       </c>
       <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s">
         <v>37</v>
-      </c>
-      <c r="C15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -823,13 +823,13 @@
         <v>1014</v>
       </c>
       <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
         <v>39</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,13 +837,13 @@
         <v>1015</v>
       </c>
       <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
         <v>41</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,13 +851,13 @@
         <v>1016</v>
       </c>
       <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
         <v>43</v>
-      </c>
-      <c r="C18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -865,13 +865,13 @@
         <v>1017</v>
       </c>
       <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" t="s">
         <v>45</v>
-      </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,13 +879,13 @@
         <v>1018</v>
       </c>
       <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>56</v>
+      </c>
+      <c r="D20" t="s">
         <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,13 +893,13 @@
         <v>1019</v>
       </c>
       <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" t="s">
         <v>49</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,13 +907,13 @@
         <v>1020</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,13 +921,13 @@
         <v>1021</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement the addLog function of the sys_log module.
</commit_message>
<xml_diff>
--- a/system_code/src/main/resources/ErrorCode.xlsx
+++ b/system_code/src/main/resources/ErrorCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -250,6 +250,14 @@
   </si>
   <si>
     <t>code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_TEST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试用错误码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -575,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -930,6 +938,20 @@
         <v>53</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1099</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement the interface of the Sys-Log module. Optimize the Sys-Code module.
</commit_message>
<xml_diff>
--- a/system_code/src/main/resources/ErrorCode.xlsx
+++ b/system_code/src/main/resources/ErrorCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -258,6 +258,14 @@
   </si>
   <si>
     <t>测试用错误码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_LOGS_NOT_FOUND</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日志读取失败</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -583,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -940,15 +948,29 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>1022</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>1099</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>58</v>
       </c>
-      <c r="C24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
oauth token & check_token & logout
</commit_message>
<xml_diff>
--- a/system_code/src/main/resources/ErrorCode.xlsx
+++ b/system_code/src/main/resources/ErrorCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
   <si>
     <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -266,6 +266,14 @@
   </si>
   <si>
     <t>日志读取失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_LOGOUT_FAILED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注销失败</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -591,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -962,15 +970,29 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>1023</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>1099</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>58</v>
       </c>
-      <c r="C25" t="s">
-        <v>3</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add auth accounts manage
</commit_message>
<xml_diff>
--- a/system_code/src/main/resources/ErrorCode.xlsx
+++ b/system_code/src/main/resources/ErrorCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -274,6 +274,14 @@
   </si>
   <si>
     <t>注销失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_NONE_ACCOUNTS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未发现任何账号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -599,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -984,15 +992,29 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>1024</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>1099</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>58</v>
       </c>
-      <c r="C26" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C27" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
role & permission & maps manage. Complete.
</commit_message>
<xml_diff>
--- a/system_code/src/main/resources/ErrorCode.xlsx
+++ b/system_code/src/main/resources/ErrorCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
   <si>
     <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -373,71 +373,87 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>指定角色不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户名无效</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_ILLEGAL_USER_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_INVALID_ROLE_NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定角色已存在或重名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_ROLE_EXIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_ACCOUNT_NOT_EXIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_ADD_ACC_ROLE_FAILED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加账户角色失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未发现任何角色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未发现任何权限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定权限不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指定权限已存在或重名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_NONE_PERMS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_PERM_NOT_EXIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_PERM_EXIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ERROR_ROLE_NOT_EXIST</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>指定角色不存在</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>用户名无效</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ERROR_ILLEGAL_USER_NAME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ERROR_INVALID_ROLE_NAME</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>指定角色已存在或重名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ERROR_ROLE_EXIST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ERROR_ACCOUNT_NOT_EXIST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ERROR_ADD_ACC_ROLE_FAILED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>添加账户角色失败</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>未发现任何角色</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>未发现任何权限</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>指定权限不存在</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>指定权限已存在或重名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ERROR_PERM_EXIST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ERROR_NONE_PERMS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ERROR_PERM_NOT_EXIST</t>
+    <t>ERROR_ADD_ROLE_PERM_FAILED</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加角色权限失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除角色权限失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ERROR_DEL_ROLE_PERM_FAILED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -763,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -896,7 +912,7 @@
         <v>1006</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8" t="s">
         <v>46</v>
@@ -1266,7 +1282,7 @@
         <v>1032</v>
       </c>
       <c r="B34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
         <v>73</v>
@@ -1314,7 +1330,7 @@
         <v>65</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1322,13 +1338,13 @@
         <v>1036</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="C38" t="s">
         <v>65</v>
       </c>
       <c r="D38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1336,13 +1352,13 @@
         <v>1037</v>
       </c>
       <c r="B39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C39" t="s">
         <v>65</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1350,13 +1366,13 @@
         <v>1038</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
         <v>65</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1364,13 +1380,13 @@
         <v>1039</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s">
         <v>65</v>
       </c>
       <c r="D41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1378,13 +1394,13 @@
         <v>1040</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
         <v>65</v>
       </c>
       <c r="D42" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1392,13 +1408,13 @@
         <v>1041</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
         <v>65</v>
       </c>
       <c r="D43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1406,26 +1422,54 @@
         <v>1042</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C44" t="s">
         <v>65</v>
       </c>
       <c r="D44" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45">
+        <v>1043</v>
+      </c>
+      <c r="B45" t="s">
+        <v>105</v>
+      </c>
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1044</v>
+      </c>
+      <c r="B46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C46" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>1999</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>50</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>3</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>